<commit_message>
update and support new Excel Record format
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Map.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19455" windowHeight="9990"/>
+    <workbookView windowWidth="28695" windowHeight="13050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136">
   <si>
     <t>Id</t>
   </si>
@@ -387,21 +387,15 @@
     <t>Maptitle100</t>
   </si>
   <si>
+    <t>Station</t>
+  </si>
+  <si>
     <t>Row</t>
   </si>
   <si>
     <t>Col</t>
   </si>
   <si>
-    <t>Index</t>
-  </si>
-  <si>
-    <t>SaveInterval</t>
-  </si>
-  <si>
-    <t>RelationValue</t>
-  </si>
-  <si>
     <t>GUID</t>
   </si>
   <si>
@@ -427,12 +421,6 @@
   </si>
   <si>
     <t>WinCount</t>
-  </si>
-  <si>
-    <t>Station</t>
-  </si>
-  <si>
-    <t>Friend</t>
   </si>
   <si>
     <t>object</t>
@@ -446,10 +434,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -467,31 +455,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -512,6 +485,74 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -519,7 +560,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -527,13 +568,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -547,13 +581,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -562,50 +589,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -638,7 +626,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -650,19 +650,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -674,19 +710,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -704,19 +728,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -728,25 +764,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -758,13 +782,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -776,49 +794,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -838,7 +826,7 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -853,7 +841,7 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -922,17 +910,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -956,16 +938,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -996,11 +978,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1024,165 +1012,180 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1191,16 +1194,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1264,7 +1264,7 @@
   <dxfs count="2">
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -1619,7 +1619,7 @@
   <sheetPr/>
   <dimension ref="A1:H107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="$A1:$XFD7"/>
     </sheetView>
   </sheetViews>
@@ -1633,185 +1633,185 @@
     <col min="7" max="7" width="9.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1" ht="27" spans="1:8">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="8" customFormat="1" ht="27" spans="1:8">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" s="4" customFormat="1" spans="1:8">
-      <c r="A2" s="8" t="s">
+    <row r="2" s="9" customFormat="1" spans="1:8">
+      <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="4" customFormat="1" spans="1:8">
-      <c r="A3" s="8" t="s">
+    <row r="3" s="9" customFormat="1" spans="1:8">
+      <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="10" t="b">
+      <c r="B3" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="C3" s="10" t="b">
+      <c r="C3" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="D3" s="10" t="b">
+      <c r="D3" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="E3" s="10" t="b">
+      <c r="E3" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="F3" s="10" t="b">
+      <c r="F3" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="G3" s="10" t="b">
+      <c r="G3" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="H3" s="10" t="b">
+      <c r="H3" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" s="4" customFormat="1" spans="1:8">
-      <c r="A4" s="8" t="s">
+    <row r="4" s="9" customFormat="1" spans="1:8">
+      <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="10" t="b">
+      <c r="B4" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="C4" s="10" t="b">
+      <c r="C4" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="D4" s="10" t="b">
+      <c r="D4" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="E4" s="10" t="b">
+      <c r="E4" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="10" t="b">
+      <c r="F4" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="G4" s="10" t="b">
+      <c r="G4" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="H4" s="10" t="b">
+      <c r="H4" s="14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" s="4" customFormat="1" spans="1:8">
-      <c r="A5" s="8" t="s">
+    <row r="5" s="9" customFormat="1" spans="1:8">
+      <c r="A5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10" t="b">
+      <c r="B5" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="C5" s="10" t="b">
+      <c r="C5" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="D5" s="10" t="b">
+      <c r="D5" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="E5" s="10" t="b">
+      <c r="E5" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="10" t="b">
+      <c r="F5" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="G5" s="10" t="b">
+      <c r="G5" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="10" t="b">
+      <c r="H5" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" s="4" customFormat="1" spans="1:8">
-      <c r="A6" s="8" t="s">
+    <row r="6" s="9" customFormat="1" spans="1:8">
+      <c r="A6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="10" t="b">
+      <c r="B6" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="C6" s="10" t="b">
+      <c r="C6" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="D6" s="10" t="b">
+      <c r="D6" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="E6" s="10" t="b">
+      <c r="E6" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="F6" s="10" t="b">
+      <c r="F6" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="G6" s="10" t="b">
+      <c r="G6" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="H6" s="10" t="b">
+      <c r="H6" s="14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="5" customFormat="1" ht="54.75" spans="1:8">
-      <c r="A7" s="11" t="s">
+    <row r="7" s="10" customFormat="1" ht="54.75" spans="1:8">
+      <c r="A7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="16" t="s">
         <v>21</v>
       </c>
     </row>
@@ -4430,163 +4430,166 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="23.125" customWidth="1"/>
-    <col min="2" max="2" width="11.875" customWidth="1"/>
-    <col min="3" max="3" width="12.625" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
-    <col min="5" max="5" width="11.625" customWidth="1"/>
-    <col min="8" max="8" width="9.375" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="10.125" customWidth="1"/>
-    <col min="13" max="14" width="12.75" customWidth="1"/>
-    <col min="15" max="15" width="14" customWidth="1"/>
-    <col min="17" max="17" width="16.5" customWidth="1"/>
-    <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="19" max="20" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="23.125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.625" style="3" customWidth="1"/>
+    <col min="6" max="7" width="9" style="3"/>
+    <col min="8" max="8" width="9.375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="19" style="3" customWidth="1"/>
+    <col min="11" max="11" width="10.125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="9" style="3"/>
+    <col min="13" max="14" width="12.75" style="3" customWidth="1"/>
+    <col min="15" max="15" width="14" style="3" customWidth="1"/>
+    <col min="16" max="16" width="9" style="3"/>
+    <col min="17" max="17" width="16.5" style="3" customWidth="1"/>
+    <col min="18" max="18" width="14" style="3" customWidth="1"/>
+    <col min="19" max="20" width="16.5" style="3" customWidth="1"/>
+    <col min="21" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" s="2" customFormat="1" spans="1:2">
+      <c r="A2" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" spans="1:2">
+      <c r="A3" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" s="2" customFormat="1" spans="1:2">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B4" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" s="2" customFormat="1" spans="1:2">
+      <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B5" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="1" spans="1:2">
+      <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B6" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" s="2" customFormat="1" spans="1:2">
+      <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="B7" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" s="2" customFormat="1" spans="1:9">
+      <c r="A8" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="J1" t="s">
+      <c r="B8" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="K1" t="s">
+      <c r="C8" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" s="2" customFormat="1" spans="1:9">
+      <c r="A9" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" s="2" customFormat="1" spans="1:2">
+      <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
-        <v>127</v>
-      </c>
-      <c r="M1" t="s">
-        <v>128</v>
-      </c>
-      <c r="N1" t="s">
-        <v>129</v>
-      </c>
-      <c r="O1" t="s">
-        <v>130</v>
-      </c>
-      <c r="P1" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>132</v>
-      </c>
-      <c r="R1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S1" t="s">
-        <v>134</v>
-      </c>
-      <c r="T1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2">
-        <v>9</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="L2" t="s">
-        <v>138</v>
-      </c>
-      <c r="M2" t="s">
-        <v>138</v>
-      </c>
-      <c r="N2" t="s">
-        <v>139</v>
-      </c>
-      <c r="O2" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>139</v>
-      </c>
-      <c r="R2" t="s">
-        <v>9</v>
-      </c>
-      <c r="S2" t="s">
-        <v>9</v>
-      </c>
-      <c r="T2" t="s">
-        <v>9</v>
+      <c r="B10" s="7" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="M1 N1 N2 P2 Q2 M3:M1048576 N3:N1048576"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576 D$1:F$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7 D10:F10 G10 G1:G7 G11:G1048576 A4:B6 D1:F7 D11:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M2 L$1:L$1048576">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B8 C8 C9 E9 F9 M10 N10 M1:M9 M11:M1048576 N1:N9 N11:N1048576"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B9 L10 A8:A9 L1:L9 L11:L1048576">
       <formula1>"int,string,float,object"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:C$1048576">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C1:C7 C11:C16374 A2:B3 B16375:C1048576">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>